<commit_message>
do i think im done?
</commit_message>
<xml_diff>
--- a/questionnaires/RBDstandardized_questionnairerCSI_FR.xlsx
+++ b/questionnaires/RBDstandardized_questionnairerCSI_FR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RBD_Resilience_guide_FR\questionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F113664A-C418-4DF5-953C-BAF3C5EC817B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17B6C13-CC3F-46C8-99BD-2E87305AE707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1545" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>type</t>
   </si>
@@ -147,6 +147,15 @@
     <t>Note for interviewers (not to read aloud): Une stratégie de rationnement dans laquelle la consommation des adultes est limitée de manière à ce que les petits enfants aient suffisamment à manger.  Dans les ménages sans enfants, la réponse devrait être zéro.</t>
   </si>
   <si>
+    <t>standardized_rCSIquestionnaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> l’indice réduit des stratégies de survie (rCSI)</t>
+  </si>
+  <si>
+    <t>Francais</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Au cours des 7 derniers jours, combien de jours votre ménage a-t-il dû
 </t>
@@ -154,18 +163,16 @@
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Consommer des aliments moins préférés et moins chers</t>
+      <t xml:space="preserve">&lt;span style="color:red"&gt;   Consommer des aliments moins préférés et moins chers &lt;/span&gt;  </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -182,19 +189,17 @@
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Emprunter de la nourriture ou compter sur l’aide des parents/amis
+      <t xml:space="preserve">&lt;span style="color:red"&gt;  Emprunter de la nourriture ou compter sur l’aide des parents/amis &lt;/span&gt;  
 </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -210,18 +215,16 @@
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Diminuer la quantité consommée pendant les repas</t>
+      <t xml:space="preserve">&lt;span style="color:red"&gt;   Diminuer la quantité consommée pendant les repas &lt;/span&gt;  </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -238,18 +241,16 @@
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Restreindre la consommation des adultes  pour nourrir les enfants</t>
+      <t xml:space="preserve">&lt;span style="color:red"&gt;   Restreindre la consommation des adultes  pour nourrir les enfants &lt;/span&gt;  </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -266,18 +267,16 @@
     <r>
       <rPr>
         <i/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Diminuer le nombre de repas par jour</t>
+      <t xml:space="preserve"> &lt;span style="color:red"&gt;  Diminuer le nombre de repas par jour &lt;/span&gt;  </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -286,21 +285,12 @@
 parce que vous n'aviez pas assez de nourriture ou de l'argent pour acheter de la nourriture ?</t>
     </r>
   </si>
-  <si>
-    <t>standardized_rCSIquestionnaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> l’indice réduit des stratégies de survie (rCSI)</t>
-  </si>
-  <si>
-    <t>Francais</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,8 +480,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,6 +509,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,7 +640,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -735,13 +738,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -757,9 +753,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -828,8 +821,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1230,7 +1246,7 @@
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.5703125" defaultRowHeight="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1291,137 +1307,136 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:14" s="70" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="72" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="73"/>
+    </row>
+    <row r="3" spans="1:14" s="74" customFormat="1" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="78" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="74" customFormat="1" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="78" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="74" customFormat="1" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="78" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="74" customFormat="1" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="D6" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="78" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="74" customFormat="1" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="41" t="s">
+      <c r="B7" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F7" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G7" s="78" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="111.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>13</v>
-      </c>
+      <c r="J7" s="79"/>
     </row>
     <row r="8" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
@@ -1435,410 +1450,410 @@
     </row>
     <row r="10" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
-      <c r="B10" s="43"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="30"/>
     </row>
     <row r="11" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="45"/>
-      <c r="J11" s="44"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="42"/>
+      <c r="J11" s="41"/>
     </row>
     <row r="12" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="46"/>
-      <c r="J12" s="50"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="43"/>
+      <c r="J12" s="46"/>
     </row>
     <row r="13" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="45"/>
-      <c r="J13" s="44"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="42"/>
+      <c r="J13" s="41"/>
     </row>
     <row r="14" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="46"/>
-      <c r="J14" s="50"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="43"/>
+      <c r="J14" s="46"/>
     </row>
     <row r="15" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="47"/>
-      <c r="J15" s="44"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="44"/>
+      <c r="J15" s="41"/>
     </row>
     <row r="16" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="47"/>
-      <c r="J16" s="44"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="44"/>
+      <c r="J16" s="41"/>
     </row>
     <row r="17" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="47"/>
-      <c r="J17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="J17" s="41"/>
     </row>
     <row r="18" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="47"/>
-      <c r="J18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="J18" s="41"/>
     </row>
     <row r="19" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
       <c r="B19" s="32"/>
-      <c r="C19" s="47"/>
-      <c r="E19" s="52"/>
+      <c r="C19" s="44"/>
+      <c r="E19" s="48"/>
       <c r="J19" s="32"/>
     </row>
     <row r="20" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
       <c r="B20" s="31"/>
-      <c r="C20" s="47"/>
+      <c r="C20" s="44"/>
       <c r="E20" s="31"/>
       <c r="J20" s="34"/>
     </row>
     <row r="21" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31"/>
       <c r="B21" s="31"/>
-      <c r="C21" s="51"/>
+      <c r="C21" s="47"/>
       <c r="E21" s="31"/>
       <c r="J21" s="34"/>
     </row>
     <row r="22" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="47"/>
-      <c r="E22" s="52"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="44"/>
+      <c r="E22" s="48"/>
       <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
-      <c r="C23" s="47"/>
+      <c r="C23" s="44"/>
       <c r="E23" s="31"/>
       <c r="J23" s="34"/>
     </row>
     <row r="24" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31"/>
       <c r="B24" s="31"/>
-      <c r="C24" s="47"/>
+      <c r="C24" s="44"/>
       <c r="E24" s="31"/>
       <c r="J24" s="34"/>
     </row>
     <row r="25" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="47"/>
-      <c r="E25" s="52"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="44"/>
+      <c r="E25" s="48"/>
       <c r="J25" s="32"/>
     </row>
     <row r="26" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="31"/>
       <c r="B26" s="31"/>
-      <c r="C26" s="47"/>
+      <c r="C26" s="44"/>
       <c r="E26" s="31"/>
       <c r="J26" s="34"/>
     </row>
     <row r="27" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="31"/>
-      <c r="C27" s="47"/>
+      <c r="C27" s="44"/>
       <c r="E27" s="31"/>
       <c r="J27" s="34"/>
     </row>
     <row r="28" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="31"/>
       <c r="B28" s="32"/>
-      <c r="C28" s="47"/>
-      <c r="E28" s="52"/>
+      <c r="C28" s="44"/>
+      <c r="E28" s="48"/>
       <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="B29" s="31"/>
-      <c r="C29" s="47"/>
+      <c r="C29" s="44"/>
       <c r="E29" s="34"/>
       <c r="J29" s="34"/>
     </row>
     <row r="30" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="47"/>
-      <c r="E30" s="55"/>
-      <c r="J30" s="55"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="44"/>
+      <c r="E30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="47"/>
-      <c r="J31" s="50"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="44"/>
+      <c r="J31" s="46"/>
     </row>
     <row r="32" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="47"/>
-      <c r="J32" s="50"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="44"/>
+      <c r="J32" s="46"/>
     </row>
     <row r="33" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="47"/>
-      <c r="E33" s="55"/>
-      <c r="J33" s="55"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="44"/>
+      <c r="E33" s="51"/>
+      <c r="J33" s="51"/>
     </row>
     <row r="34" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="47"/>
-      <c r="E34" s="44"/>
-      <c r="J34" s="50"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="44"/>
+      <c r="E34" s="41"/>
+      <c r="J34" s="46"/>
     </row>
     <row r="35" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="31"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="47"/>
-      <c r="E35" s="44"/>
-      <c r="J35" s="50"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="44"/>
+      <c r="E35" s="41"/>
+      <c r="J35" s="46"/>
     </row>
     <row r="36" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="47"/>
-      <c r="E36" s="55"/>
-      <c r="J36" s="55"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="44"/>
+      <c r="E36" s="51"/>
+      <c r="J36" s="51"/>
     </row>
     <row r="37" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="47"/>
-      <c r="E37" s="44"/>
-      <c r="J37" s="50"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="44"/>
+      <c r="E37" s="41"/>
+      <c r="J37" s="46"/>
     </row>
     <row r="38" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="47"/>
-      <c r="E38" s="44"/>
-      <c r="J38" s="50"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="44"/>
+      <c r="E38" s="41"/>
+      <c r="J38" s="46"/>
     </row>
     <row r="39" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="54"/>
-      <c r="C39" s="47"/>
-      <c r="E39" s="55"/>
-      <c r="J39" s="55"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="44"/>
+      <c r="E39" s="51"/>
+      <c r="J39" s="51"/>
     </row>
     <row r="40" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="47"/>
-      <c r="J40" s="57"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="44"/>
+      <c r="J40" s="53"/>
     </row>
     <row r="41" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="47"/>
-      <c r="J41" s="57"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="44"/>
+      <c r="J41" s="53"/>
     </row>
     <row r="42" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="47"/>
-      <c r="J42" s="44"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="41"/>
+      <c r="C42" s="44"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
       <c r="B43" s="32"/>
-      <c r="C43" s="47"/>
+      <c r="C43" s="44"/>
       <c r="E43" s="31"/>
       <c r="J43" s="31"/>
     </row>
     <row r="44" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="47"/>
-      <c r="E44" s="61"/>
-      <c r="J44" s="60"/>
+      <c r="A44" s="55"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="44"/>
+      <c r="E44" s="57"/>
+      <c r="J44" s="56"/>
     </row>
     <row r="45" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="44"/>
-      <c r="B45" s="62"/>
-      <c r="C45" s="47"/>
-      <c r="E45" s="44"/>
-      <c r="J45" s="56"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="44"/>
+      <c r="E45" s="41"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="44"/>
-      <c r="B46" s="63"/>
-      <c r="C46" s="47"/>
-      <c r="E46" s="56"/>
-      <c r="J46" s="56"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="44"/>
+      <c r="E46" s="52"/>
+      <c r="J46" s="52"/>
     </row>
     <row r="47" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="47"/>
-      <c r="E47" s="56"/>
-      <c r="J47" s="56"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="44"/>
+      <c r="E47" s="52"/>
+      <c r="J47" s="52"/>
     </row>
     <row r="48" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="44"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="47"/>
-      <c r="E48" s="44"/>
-      <c r="J48" s="56"/>
+      <c r="A48" s="41"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="44"/>
+      <c r="E48" s="41"/>
+      <c r="J48" s="52"/>
     </row>
     <row r="49" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="44"/>
-      <c r="B49" s="58"/>
-      <c r="C49" s="47"/>
-      <c r="E49" s="56"/>
-      <c r="J49" s="56"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="44"/>
+      <c r="E49" s="52"/>
+      <c r="J49" s="52"/>
     </row>
     <row r="50" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
-      <c r="B50" s="58"/>
-      <c r="C50" s="47"/>
-      <c r="E50" s="56"/>
-      <c r="J50" s="56"/>
+      <c r="B50" s="54"/>
+      <c r="C50" s="44"/>
+      <c r="E50" s="52"/>
+      <c r="J50" s="52"/>
     </row>
     <row r="51" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="31"/>
       <c r="B51" s="32"/>
-      <c r="C51" s="47"/>
+      <c r="C51" s="44"/>
       <c r="E51" s="31"/>
       <c r="J51" s="31"/>
     </row>
     <row r="52" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
       <c r="B52" s="31"/>
-      <c r="C52" s="47"/>
+      <c r="C52" s="44"/>
       <c r="E52" s="31"/>
-      <c r="J52" s="59"/>
+      <c r="J52" s="55"/>
     </row>
     <row r="53" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
       <c r="B53" s="31"/>
-      <c r="C53" s="47"/>
+      <c r="C53" s="44"/>
       <c r="E53" s="31"/>
-      <c r="J53" s="59"/>
+      <c r="J53" s="55"/>
     </row>
     <row r="54" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="54"/>
-      <c r="C54" s="47"/>
-      <c r="E54" s="44"/>
+      <c r="A54" s="41"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="44"/>
+      <c r="E54" s="41"/>
       <c r="J54" s="37"/>
     </row>
     <row r="55" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="44"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="47"/>
-      <c r="E55" s="44"/>
+      <c r="A55" s="41"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="44"/>
+      <c r="E55" s="41"/>
       <c r="J55" s="37"/>
     </row>
     <row r="56" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="31"/>
-      <c r="B56" s="44"/>
-      <c r="C56" s="47"/>
-      <c r="E56" s="44"/>
+      <c r="B56" s="41"/>
+      <c r="C56" s="44"/>
+      <c r="E56" s="41"/>
       <c r="J56" s="37"/>
     </row>
     <row r="57" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="31"/>
       <c r="B57" s="32"/>
-      <c r="C57" s="47"/>
+      <c r="C57" s="44"/>
       <c r="E57" s="31"/>
       <c r="J57" s="31"/>
     </row>
     <row r="58" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="31"/>
-      <c r="B58" s="64"/>
-      <c r="C58" s="47"/>
+      <c r="B58" s="60"/>
+      <c r="C58" s="44"/>
       <c r="E58" s="31"/>
-      <c r="J58" s="59"/>
+      <c r="J58" s="55"/>
     </row>
     <row r="59" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="31"/>
-      <c r="B59" s="64"/>
-      <c r="C59" s="47"/>
+      <c r="B59" s="60"/>
+      <c r="C59" s="44"/>
       <c r="E59" s="31"/>
-      <c r="J59" s="59"/>
+      <c r="J59" s="55"/>
     </row>
     <row r="60" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="31"/>
-      <c r="B60" s="53"/>
-      <c r="C60" s="47"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="44"/>
       <c r="E60" s="31"/>
-      <c r="J60" s="59"/>
+      <c r="J60" s="55"/>
     </row>
     <row r="61" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="31"/>
-      <c r="B61" s="64"/>
-      <c r="C61" s="47"/>
-      <c r="J61" s="59"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="44"/>
+      <c r="J61" s="55"/>
     </row>
     <row r="62" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="31"/>
-      <c r="B62" s="64"/>
-      <c r="C62" s="47"/>
-      <c r="J62" s="59"/>
+      <c r="B62" s="60"/>
+      <c r="C62" s="44"/>
+      <c r="J62" s="55"/>
     </row>
     <row r="63" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="31"/>
-      <c r="B63" s="53"/>
-      <c r="C63" s="47"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="44"/>
       <c r="E63" s="31"/>
-      <c r="J63" s="44"/>
+      <c r="J63" s="41"/>
     </row>
     <row r="64" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="31"/>
-      <c r="B64" s="64"/>
-      <c r="C64" s="47"/>
-      <c r="J64" s="59"/>
+      <c r="B64" s="60"/>
+      <c r="C64" s="44"/>
+      <c r="J64" s="55"/>
     </row>
     <row r="65" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="31"/>
-      <c r="B65" s="43"/>
-      <c r="C65" s="47"/>
-      <c r="J65" s="59"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="44"/>
+      <c r="J65" s="55"/>
     </row>
     <row r="66" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="31"/>
-      <c r="B66" s="43"/>
-      <c r="C66" s="47"/>
-      <c r="J66" s="44"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="44"/>
+      <c r="J66" s="41"/>
     </row>
     <row r="67" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="31"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="47"/>
-      <c r="J67" s="44"/>
+      <c r="B67" s="40"/>
+      <c r="C67" s="44"/>
+      <c r="J67" s="41"/>
     </row>
     <row r="68" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="31"/>
-      <c r="B68" s="43"/>
-      <c r="C68" s="47"/>
-      <c r="J68" s="44"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="44"/>
+      <c r="J68" s="41"/>
     </row>
     <row r="69" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="31"/>
-      <c r="B69" s="43"/>
-      <c r="C69" s="47"/>
-      <c r="J69" s="44"/>
+      <c r="B69" s="40"/>
+      <c r="C69" s="44"/>
+      <c r="J69" s="41"/>
     </row>
     <row r="70" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="31"/>
-      <c r="B70" s="43"/>
-      <c r="C70" s="47"/>
-      <c r="J70" s="44"/>
+      <c r="B70" s="40"/>
+      <c r="C70" s="44"/>
+      <c r="J70" s="41"/>
     </row>
     <row r="71" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="31"/>
-      <c r="B71" s="47"/>
+      <c r="B71" s="44"/>
       <c r="C71" s="20"/>
     </row>
     <row r="72" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1884,11 +1899,11 @@
     </row>
     <row r="82" spans="2:3" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="18"/>
-      <c r="C82" s="65"/>
+      <c r="C82" s="61"/>
     </row>
     <row r="83" spans="2:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="18"/>
-      <c r="C83" s="66"/>
+      <c r="C83" s="62"/>
     </row>
     <row r="84" spans="2:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="18"/>
@@ -2038,13 +2053,13 @@
       <c r="J124" s="34"/>
     </row>
     <row r="125" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="67"/>
+      <c r="A125" s="63"/>
       <c r="B125" s="36"/>
       <c r="J125" s="34"/>
     </row>
     <row r="126" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="31"/>
-      <c r="B126" s="53"/>
+      <c r="B126" s="49"/>
       <c r="J126" s="32"/>
     </row>
     <row r="127" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2053,7 +2068,7 @@
       <c r="J127" s="34"/>
     </row>
     <row r="128" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="67"/>
+      <c r="A128" s="63"/>
       <c r="B128" s="36"/>
       <c r="J128" s="34"/>
     </row>
@@ -2068,74 +2083,74 @@
       <c r="J130" s="34"/>
     </row>
     <row r="131" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="44"/>
-      <c r="B131" s="54"/>
-      <c r="J131" s="55"/>
+      <c r="A131" s="41"/>
+      <c r="B131" s="50"/>
+      <c r="J131" s="51"/>
     </row>
     <row r="132" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="44"/>
-      <c r="B132" s="44"/>
-      <c r="J132" s="50"/>
+      <c r="A132" s="41"/>
+      <c r="B132" s="41"/>
+      <c r="J132" s="46"/>
     </row>
     <row r="133" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="67"/>
+      <c r="A133" s="63"/>
       <c r="B133" s="18"/>
-      <c r="J133" s="50"/>
+      <c r="J133" s="46"/>
     </row>
     <row r="134" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="44"/>
-      <c r="B134" s="54"/>
-      <c r="J134" s="55"/>
+      <c r="A134" s="41"/>
+      <c r="B134" s="50"/>
+      <c r="J134" s="51"/>
     </row>
     <row r="135" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="44"/>
-      <c r="B135" s="44"/>
-      <c r="J135" s="50"/>
+      <c r="A135" s="41"/>
+      <c r="B135" s="41"/>
+      <c r="J135" s="46"/>
     </row>
     <row r="136" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="67"/>
-      <c r="B136" s="44"/>
-      <c r="J136" s="50"/>
+      <c r="A136" s="63"/>
+      <c r="B136" s="41"/>
+      <c r="J136" s="46"/>
     </row>
     <row r="137" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="44"/>
-      <c r="B137" s="54"/>
-      <c r="J137" s="55"/>
+      <c r="A137" s="41"/>
+      <c r="B137" s="50"/>
+      <c r="J137" s="51"/>
     </row>
     <row r="138" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="44"/>
-      <c r="B138" s="44"/>
-      <c r="J138" s="50"/>
+      <c r="A138" s="41"/>
+      <c r="B138" s="41"/>
+      <c r="J138" s="46"/>
     </row>
     <row r="139" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="67"/>
+      <c r="A139" s="63"/>
       <c r="B139" s="18"/>
-      <c r="J139" s="50"/>
+      <c r="J139" s="46"/>
     </row>
     <row r="140" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="44"/>
-      <c r="B140" s="54"/>
-      <c r="J140" s="55"/>
+      <c r="A140" s="41"/>
+      <c r="B140" s="50"/>
+      <c r="J140" s="51"/>
     </row>
     <row r="141" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="44"/>
-      <c r="B141" s="56"/>
-      <c r="J141" s="57"/>
+      <c r="A141" s="41"/>
+      <c r="B141" s="52"/>
+      <c r="J141" s="53"/>
     </row>
     <row r="142" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="67"/>
+      <c r="A142" s="63"/>
       <c r="B142" s="18"/>
-      <c r="J142" s="57"/>
+      <c r="J142" s="53"/>
     </row>
     <row r="143" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="44"/>
-      <c r="B143" s="44"/>
-      <c r="J143" s="44"/>
+      <c r="A143" s="41"/>
+      <c r="B143" s="41"/>
+      <c r="J143" s="41"/>
     </row>
     <row r="144" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="44"/>
-      <c r="B144" s="44"/>
-      <c r="J144" s="44"/>
+      <c r="A144" s="41"/>
+      <c r="B144" s="41"/>
+      <c r="J144" s="41"/>
     </row>
     <row r="145" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="31"/>
@@ -2143,39 +2158,39 @@
       <c r="J145" s="31"/>
     </row>
     <row r="146" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="59"/>
-      <c r="B146" s="60"/>
-      <c r="J146" s="60"/>
+      <c r="A146" s="55"/>
+      <c r="B146" s="56"/>
+      <c r="J146" s="56"/>
     </row>
     <row r="147" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="44"/>
-      <c r="B147" s="62"/>
-      <c r="J147" s="56"/>
+      <c r="A147" s="41"/>
+      <c r="B147" s="58"/>
+      <c r="J147" s="52"/>
     </row>
     <row r="148" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="44"/>
-      <c r="B148" s="63"/>
-      <c r="J148" s="56"/>
+      <c r="A148" s="41"/>
+      <c r="B148" s="59"/>
+      <c r="J148" s="52"/>
     </row>
     <row r="149" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="67"/>
-      <c r="B149" s="63"/>
-      <c r="J149" s="56"/>
+      <c r="A149" s="63"/>
+      <c r="B149" s="59"/>
+      <c r="J149" s="52"/>
     </row>
     <row r="150" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="44"/>
-      <c r="B150" s="62"/>
-      <c r="J150" s="56"/>
+      <c r="A150" s="41"/>
+      <c r="B150" s="58"/>
+      <c r="J150" s="52"/>
     </row>
     <row r="151" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="44"/>
-      <c r="B151" s="58"/>
-      <c r="J151" s="56"/>
+      <c r="A151" s="41"/>
+      <c r="B151" s="54"/>
+      <c r="J151" s="52"/>
     </row>
     <row r="152" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="67"/>
-      <c r="B152" s="58"/>
-      <c r="J152" s="56"/>
+      <c r="A152" s="63"/>
+      <c r="B152" s="54"/>
+      <c r="J152" s="52"/>
     </row>
     <row r="153" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="31"/>
@@ -2185,26 +2200,26 @@
     <row r="154" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="31"/>
       <c r="B154" s="31"/>
-      <c r="J154" s="59"/>
+      <c r="J154" s="55"/>
     </row>
     <row r="155" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="67"/>
+      <c r="A155" s="63"/>
       <c r="B155" s="18"/>
-      <c r="J155" s="59"/>
+      <c r="J155" s="55"/>
     </row>
     <row r="156" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="44"/>
-      <c r="B156" s="54"/>
+      <c r="A156" s="41"/>
+      <c r="B156" s="50"/>
       <c r="J156" s="37"/>
     </row>
     <row r="157" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="44"/>
-      <c r="B157" s="44"/>
+      <c r="A157" s="41"/>
+      <c r="B157" s="41"/>
       <c r="J157" s="37"/>
     </row>
     <row r="158" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="67"/>
-      <c r="B158" s="44"/>
+      <c r="A158" s="63"/>
+      <c r="B158" s="41"/>
       <c r="J158" s="37"/>
     </row>
     <row r="159" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2214,141 +2229,141 @@
     </row>
     <row r="160" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="31"/>
-      <c r="B160" s="64"/>
-      <c r="J160" s="59"/>
+      <c r="B160" s="60"/>
+      <c r="J160" s="55"/>
     </row>
     <row r="161" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="67"/>
+      <c r="A161" s="63"/>
       <c r="B161" s="18"/>
-      <c r="J161" s="59"/>
+      <c r="J161" s="55"/>
     </row>
     <row r="162" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="31"/>
-      <c r="B162" s="53"/>
-      <c r="J162" s="59"/>
+      <c r="B162" s="49"/>
+      <c r="J162" s="55"/>
     </row>
     <row r="163" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="31"/>
-      <c r="B163" s="64"/>
-      <c r="J163" s="59"/>
+      <c r="B163" s="60"/>
+      <c r="J163" s="55"/>
     </row>
     <row r="164" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="67"/>
+      <c r="A164" s="63"/>
       <c r="B164" s="18"/>
-      <c r="J164" s="59"/>
+      <c r="J164" s="55"/>
     </row>
     <row r="165" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="31"/>
-      <c r="B165" s="64"/>
-      <c r="J165" s="59"/>
+      <c r="B165" s="60"/>
+      <c r="J165" s="55"/>
     </row>
     <row r="166" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="31"/>
-      <c r="B166" s="64"/>
-      <c r="J166" s="59"/>
+      <c r="B166" s="60"/>
+      <c r="J166" s="55"/>
     </row>
     <row r="167" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="67"/>
+      <c r="A167" s="63"/>
       <c r="B167" s="18"/>
-      <c r="J167" s="59"/>
+      <c r="J167" s="55"/>
     </row>
     <row r="168" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="68"/>
-      <c r="B168" s="69"/>
+      <c r="A168" s="64"/>
+      <c r="B168" s="65"/>
     </row>
     <row r="170" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="18"/>
     </row>
     <row r="171" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J171" s="59"/>
+      <c r="J171" s="55"/>
     </row>
     <row r="172" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J172" s="59"/>
+      <c r="J172" s="55"/>
     </row>
     <row r="176" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="18"/>
     </row>
     <row r="177" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J177" s="59"/>
+      <c r="J177" s="55"/>
     </row>
     <row r="178" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J178" s="59"/>
+      <c r="J178" s="55"/>
     </row>
     <row r="182" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="18"/>
     </row>
     <row r="183" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J183" s="59"/>
+      <c r="J183" s="55"/>
     </row>
     <row r="184" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J184" s="59"/>
+      <c r="J184" s="55"/>
     </row>
     <row r="187" spans="2:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="188" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="18"/>
     </row>
     <row r="189" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J189" s="59"/>
+      <c r="J189" s="55"/>
     </row>
     <row r="190" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J190" s="59"/>
+      <c r="J190" s="55"/>
     </row>
     <row r="194" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="18"/>
     </row>
     <row r="195" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J195" s="59"/>
+      <c r="J195" s="55"/>
     </row>
     <row r="196" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J196" s="59"/>
+      <c r="J196" s="55"/>
     </row>
     <row r="199" spans="2:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="200" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="18"/>
     </row>
     <row r="201" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J201" s="59"/>
+      <c r="J201" s="55"/>
     </row>
     <row r="202" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J202" s="59"/>
+      <c r="J202" s="55"/>
     </row>
     <row r="206" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="18"/>
     </row>
     <row r="207" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J207" s="59"/>
+      <c r="J207" s="55"/>
     </row>
     <row r="208" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J208" s="59"/>
+      <c r="J208" s="55"/>
     </row>
     <row r="211" spans="2:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="212" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="18"/>
     </row>
     <row r="213" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J213" s="59"/>
+      <c r="J213" s="55"/>
     </row>
     <row r="214" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J214" s="59"/>
+      <c r="J214" s="55"/>
     </row>
     <row r="218" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B218" s="18"/>
     </row>
     <row r="219" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J219" s="59"/>
+      <c r="J219" s="55"/>
     </row>
     <row r="220" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J220" s="59"/>
+      <c r="J220" s="55"/>
     </row>
     <row r="223" spans="2:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="224" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B224" s="18"/>
     </row>
     <row r="225" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J225" s="59"/>
+      <c r="J225" s="55"/>
     </row>
     <row r="226" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J226" s="59"/>
+      <c r="J226" s="55"/>
     </row>
     <row r="230" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B230" s="18"/>
@@ -2357,10 +2372,10 @@
       <c r="B231" s="18"/>
     </row>
     <row r="232" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B232" s="70"/>
+      <c r="B232" s="66"/>
     </row>
     <row r="233" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B233" s="70"/>
+      <c r="B233" s="66"/>
     </row>
     <row r="234" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B234" s="18"/>
@@ -2440,40 +2455,40 @@
     <row r="260" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B260" s="18"/>
     </row>
-    <row r="263" spans="1:8" s="44" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B263" s="71"/>
-      <c r="C263" s="72"/>
-      <c r="D263" s="72"/>
-      <c r="E263" s="73"/>
-      <c r="F263" s="50"/>
-      <c r="H263" s="73"/>
-    </row>
-    <row r="264" spans="1:8" s="44" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" s="41" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B263" s="67"/>
+      <c r="C263" s="68"/>
+      <c r="D263" s="68"/>
+      <c r="E263" s="69"/>
+      <c r="F263" s="46"/>
+      <c r="H263" s="69"/>
+    </row>
+    <row r="264" spans="1:8" s="41" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="31"/>
       <c r="B264" s="32"/>
       <c r="C264" s="33"/>
     </row>
-    <row r="265" spans="1:8" s="44" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" s="41" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="31"/>
       <c r="B265" s="32"/>
       <c r="C265" s="33"/>
     </row>
-    <row r="266" spans="1:8" s="44" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" s="41" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="31"/>
       <c r="B266" s="32"/>
       <c r="C266" s="33"/>
     </row>
-    <row r="267" spans="1:8" s="44" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" s="41" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="31"/>
       <c r="B267" s="32"/>
       <c r="C267" s="33"/>
     </row>
-    <row r="268" spans="1:8" s="44" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" s="41" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="31"/>
       <c r="B268" s="32"/>
       <c r="C268" s="33"/>
     </row>
-    <row r="269" spans="1:8" s="44" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" s="41" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="31"/>
       <c r="B269" s="32"/>
       <c r="C269" s="33"/>
@@ -2567,7 +2582,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13"/>
-      <c r="C13" s="42"/>
+      <c r="C13" s="39"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14"/>
@@ -4757,13 +4772,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -4785,21 +4800,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D9E21B46B6510944ACCC1A9E9D09B45B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b02bb79e95f874242395453643404308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0aae8104-2775-47bf-a616-40d8eadd5188" xmlns:ns4="8dd5283b-55c2-4f3c-990c-ab18dea8320e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d6c59ce88ebf0eb87405994d35ea81e" ns3:_="" ns4:_="">
     <xsd:import namespace="0aae8104-2775-47bf-a616-40d8eadd5188"/>
@@ -5016,32 +5016,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50755B8E-7E00-4BEC-BA51-4E6E4B22BCE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="0aae8104-2775-47bf-a616-40d8eadd5188"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8dd5283b-55c2-4f3c-990c-ab18dea8320e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D66C5643-24C7-4807-886B-BE44B695FAF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF46C5BC-2557-46C4-92CA-B3C69F93D2EF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5058,4 +5048,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D66C5643-24C7-4807-886B-BE44B695FAF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50755B8E-7E00-4BEC-BA51-4E6E4B22BCE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="0aae8104-2775-47bf-a616-40d8eadd5188"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8dd5283b-55c2-4f3c-990c-ab18dea8320e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>